<commit_message>
single qry upload fix
</commit_message>
<xml_diff>
--- a/Backend/uploads/Test Data 3.xlsx
+++ b/Backend/uploads/Test Data 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Raghav/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7406267B-113C-054F-8B2B-6F60D9750F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EB6EB2-2A82-4F4A-A840-65B277D08FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{64139431-5CF8-457C-8E51-C564E81C114F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Sl.No</t>
   </si>
@@ -756,7 +756,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -807,9 +807,7 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="E2" s="2"/>
       <c r="F2" s="2">
         <v>1</v>
       </c>

</xml_diff>